<commit_message>
success task Arif 0829_8 filename ( 20.0657 )
</commit_message>
<xml_diff>
--- a/Arif 0829_8/Arif 0829_8.xlsx
+++ b/Arif 0829_8/Arif 0829_8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Scraping\Don Osterloh\Scraping data\Arif 0829_8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D38995-1A2A-44D8-8A28-B909092FBEE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E101F108-EC23-4473-866F-D9EC87B47AAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
   <si>
     <r>
       <rPr>
@@ -108,16 +108,6 @@
         <color rgb="FF000000"/>
         <rFont val="Eurostile"/>
       </rPr>
-      <t>Pull all going back to 2014</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Eurostile"/>
-      </rPr>
       <t>Members of Parliament</t>
     </r>
   </si>
@@ -325,6 +315,12 @@
   </si>
   <si>
     <t>Aug 31 2023</t>
+  </si>
+  <si>
+    <t>Sep 01 2023</t>
+  </si>
+  <si>
+    <t>Pull all going back to 2014</t>
   </si>
 </sst>
 </file>
@@ -334,12 +330,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000_);[Red]\(0.0000\)"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -477,101 +480,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -586,7 +574,25 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1080,8 +1086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1125,19 +1131,19 @@
         <v>20.065000000000001</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="24">
         <v>4</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
@@ -1148,19 +1154,19 @@
         <v>20.065100000000001</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="24">
         <v>28</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
@@ -1171,15 +1177,15 @@
         <v>20.065200000000001</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="29"/>
       <c r="D4" s="29"/>
       <c r="E4" s="30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G4" s="28"/>
       <c r="H4" s="28"/>
@@ -1190,17 +1196,17 @@
         <v>20.065300000000001</v>
       </c>
       <c r="B5" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="34" t="s">
         <v>51</v>
-      </c>
-      <c r="C5" s="34" t="s">
-        <v>52</v>
       </c>
       <c r="D5" s="34"/>
       <c r="E5" s="35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G5" s="33"/>
       <c r="H5" s="33"/>
@@ -1211,19 +1217,19 @@
         <v>20.0654</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="24">
         <v>7</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G6" s="23"/>
       <c r="H6" s="23"/>
@@ -1234,77 +1240,81 @@
         <v>20.0655</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="24">
         <v>6</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G7" s="23"/>
       <c r="H7" s="23"/>
       <c r="I7" s="23"/>
     </row>
-    <row r="8" spans="1:9" s="17" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A8" s="14">
+    <row r="8" spans="1:9" s="37" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A8" s="22">
         <v>20.0656</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="24">
+        <v>1</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+    </row>
+    <row r="9" spans="1:9" s="17" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A9" s="14">
+        <v>20.0657</v>
+      </c>
+      <c r="B9" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-    </row>
-    <row r="9" spans="1:9" s="9" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A9" s="7">
-        <v>20.0657</v>
-      </c>
-      <c r="B9" s="8" t="s">
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
+      <c r="F9" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:9" s="9" customFormat="1" ht="27.75" customHeight="1">
       <c r="A10" s="7">
         <v>20.065799999999999</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
       <c r="E10" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>7</v>
@@ -1318,18 +1328,18 @@
         <v>20.065899999999999</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
       <c r="E11" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>7</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
@@ -1339,16 +1349,16 @@
         <v>20.066099999999999</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="19"/>
       <c r="D12" s="19"/>
       <c r="E12" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
@@ -1358,16 +1368,16 @@
         <v>20.066199999999998</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="19"/>
       <c r="E13" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
@@ -1377,18 +1387,18 @@
         <v>20.0718</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
       <c r="E14" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>7</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
@@ -1398,12 +1408,12 @@
         <v>20.073</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
       <c r="E15" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>7</v>
@@ -1417,12 +1427,12 @@
         <v>20.0731</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
       <c r="E16" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>7</v>
@@ -1436,12 +1446,12 @@
         <v>20.0732</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
       <c r="E17" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>7</v>
@@ -1455,12 +1465,12 @@
         <v>20.0733</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
       <c r="E18" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>7</v>
@@ -1474,12 +1484,12 @@
         <v>20.073399999999999</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
       <c r="E19" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>7</v>
@@ -1493,12 +1503,12 @@
         <v>20.073499999999999</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
       <c r="E20" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>7</v>
@@ -1512,12 +1522,12 @@
         <v>20.073599999999999</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
       <c r="E21" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
success task Arif 0829_8 filename 20.0734
</commit_message>
<xml_diff>
--- a/Arif 0829_8/Arif 0829_8.xlsx
+++ b/Arif 0829_8/Arif 0829_8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Scraping\Don Osterloh\Scraping data\Arif 0829_8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E07423D-B6EF-4BC8-857F-BDF70A54F97A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B888422D-044E-454B-AE51-6818BDD2E802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="57">
   <si>
     <r>
       <rPr>
@@ -108,77 +108,7 @@
         <color rgb="FF000000"/>
         <rFont val="Eurostile"/>
       </rPr>
-      <t>NZ Council</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Eurostile"/>
-      </rPr>
       <t>Our Team</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Eurostile"/>
-      </rPr>
-      <t>Check back for non-elected people section of this site. No point in capturing elected officials, we'll get those elsewhere.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Eurostile"/>
-      </rPr>
-      <t>Our People</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Eurostile"/>
-      </rPr>
-      <t>PDF download</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Eurostile"/>
-      </rPr>
-      <t>Chief Executive &amp; Directors</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Eurostile"/>
-      </rPr>
-      <t>City Council - Councillors</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Eurostile"/>
-      </rPr>
-      <t>City Council - Representatives</t>
     </r>
   </si>
   <si>
@@ -315,6 +245,30 @@
   <si>
     <t>Members of Parliament</t>
   </si>
+  <si>
+    <t>NZ Council</t>
+  </si>
+  <si>
+    <t>Our People</t>
+  </si>
+  <si>
+    <t>Chief Executive &amp; Directors</t>
+  </si>
+  <si>
+    <t>PDF download</t>
+  </si>
+  <si>
+    <t>City Council - Councillors</t>
+  </si>
+  <si>
+    <t>City Council - Representatives</t>
+  </si>
+  <si>
+    <t>Sep 02 2023</t>
+  </si>
+  <si>
+    <t>Mayor</t>
+  </si>
 </sst>
 </file>
 
@@ -323,7 +277,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000_);[Red]\(0.0000\)"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -353,6 +307,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Eurostile"/>
@@ -380,13 +355,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Eurostile"/>
-    </font>
-    <font>
-      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -395,6 +370,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -403,24 +386,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Eurostile"/>
+    </font>
+    <font>
+      <b/>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -480,119 +455,131 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1089,16 +1076,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.7109375" style="12" customWidth="1"/>
     <col min="2" max="2" width="40.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="21" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="16" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" style="16" customWidth="1"/>
     <col min="5" max="5" width="78.28515625" customWidth="1"/>
     <col min="6" max="6" width="43.42578125" customWidth="1"/>
     <col min="7" max="9" width="16.85546875" customWidth="1"/>
@@ -1129,317 +1116,337 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="26" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A2" s="22">
+    <row r="2" spans="1:9" s="21" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A2" s="17">
         <v>20.065000000000001</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="19">
+        <v>4</v>
+      </c>
+      <c r="D2" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="24">
-        <v>4</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+    </row>
+    <row r="3" spans="1:9" s="21" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A3" s="17">
+        <v>20.065100000000001</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="19">
+        <v>28</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+    </row>
+    <row r="4" spans="1:9" s="26" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A4" s="22">
+        <v>20.065200000000001</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+    </row>
+    <row r="5" spans="1:9" s="31" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A5" s="27">
+        <v>20.065300000000001</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="29"/>
+      <c r="E5" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+    </row>
+    <row r="6" spans="1:9" s="21" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A6" s="17">
+        <v>20.0654</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="19">
+        <v>7</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+    </row>
+    <row r="7" spans="1:9" s="21" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A7" s="17">
+        <v>20.0655</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="19">
+        <v>6</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+    </row>
+    <row r="8" spans="1:9" s="32" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A8" s="17">
+        <v>20.0656</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="19">
+        <v>1</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+    </row>
+    <row r="9" spans="1:9" s="33" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A9" s="17">
+        <v>20.0657</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="19">
+        <v>2</v>
+      </c>
+      <c r="D9" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-    </row>
-    <row r="3" spans="1:9" s="26" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A3" s="22">
-        <v>20.065100000000001</v>
-      </c>
-      <c r="B3" s="23" t="s">
+      <c r="E9" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="24">
-        <v>28</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="23" t="s">
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+    </row>
+    <row r="10" spans="1:9" s="34" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A10" s="17">
+        <v>20.065799999999999</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="19">
+        <v>119</v>
+      </c>
+      <c r="D10" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-    </row>
-    <row r="4" spans="1:9" s="31" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A4" s="27">
-        <v>20.065200000000001</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="28" t="s">
+      <c r="E10" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+    </row>
+    <row r="11" spans="1:9" s="35" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A11" s="17">
+        <v>20.065899999999999</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="19">
+        <v>22</v>
+      </c>
+      <c r="D11" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-    </row>
-    <row r="5" spans="1:9" s="36" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A5" s="32">
-        <v>20.065300000000001</v>
-      </c>
-      <c r="B5" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" s="34"/>
-      <c r="E5" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-    </row>
-    <row r="6" spans="1:9" s="26" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A6" s="22">
-        <v>20.0654</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="24">
-        <v>7</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-    </row>
-    <row r="7" spans="1:9" s="26" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A7" s="22">
-        <v>20.0655</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="24">
-        <v>6</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" s="25" t="s">
+      <c r="E11" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-    </row>
-    <row r="8" spans="1:9" s="37" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A8" s="22">
-        <v>20.0656</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="24">
-        <v>1</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" s="25" t="s">
+      <c r="F11" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-    </row>
-    <row r="9" spans="1:9" s="38" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A9" s="22">
-        <v>20.0657</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="24">
-        <v>2</v>
-      </c>
-      <c r="D9" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="G9" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-    </row>
-    <row r="10" spans="1:9" s="17" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A10" s="14">
-        <v>20.065799999999999</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-    </row>
-    <row r="11" spans="1:9" s="9" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A11" s="7">
-        <v>20.065899999999999</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
     </row>
     <row r="12" spans="1:9" s="9" customFormat="1" ht="27.75" customHeight="1">
       <c r="A12" s="7">
         <v>20.066099999999999</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
+        <v>8</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
       <c r="E12" s="13" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="10" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
     </row>
-    <row r="13" spans="1:9" s="9" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A13" s="7">
+    <row r="13" spans="1:9" s="35" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A13" s="17">
         <v>20.066199999999998</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="10" t="s">
+      <c r="B13" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="19">
         <v>10</v>
       </c>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-    </row>
-    <row r="14" spans="1:9" s="9" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A14" s="7">
+      <c r="D13" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="18"/>
+      <c r="G13" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+    </row>
+    <row r="14" spans="1:9" s="35" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A14" s="17">
         <v>20.0718</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-    </row>
-    <row r="15" spans="1:9" s="9" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A15" s="7">
+      <c r="B14" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="19">
+        <v>13</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+    </row>
+    <row r="15" spans="1:9" s="35" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A15" s="17">
         <v>20.073</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
+      <c r="B15" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="19">
+        <v>6</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
     </row>
     <row r="16" spans="1:9" s="9" customFormat="1" ht="27.75" customHeight="1">
       <c r="A16" s="7">
         <v>20.0731</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
+        <v>32</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
       <c r="E16" s="13" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>7</v>
@@ -1448,74 +1455,82 @@
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
     </row>
-    <row r="17" spans="1:9" s="9" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A17" s="7">
+    <row r="17" spans="1:9" s="35" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A17" s="17">
         <v>20.0732</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-    </row>
-    <row r="18" spans="1:9" s="9" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A18" s="7">
+      <c r="B17" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="19">
+        <v>15</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+    </row>
+    <row r="18" spans="1:9" s="42" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A18" s="17">
         <v>20.0733</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-    </row>
-    <row r="19" spans="1:9" s="9" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A19" s="7">
+      <c r="B18" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="19">
+        <v>2</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+    </row>
+    <row r="19" spans="1:9" s="41" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A19" s="37">
         <v>20.073399999999999</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
+      <c r="B19" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
     </row>
     <row r="20" spans="1:9" s="9" customFormat="1" ht="27.75" customHeight="1">
       <c r="A20" s="7">
         <v>20.073499999999999</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
+        <v>10</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
       <c r="E20" s="13" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>7</v>
@@ -1529,12 +1544,12 @@
         <v>20.073599999999999</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
+        <v>9</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
       <c r="E21" s="13" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>7</v>
@@ -1546,8 +1561,8 @@
     <row r="22" spans="1:9">
       <c r="A22" s="11"/>
       <c r="B22" s="4"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
       <c r="E22" s="5"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>

</xml_diff>

<commit_message>
success task Arif 0829_8 filename 20.0733
</commit_message>
<xml_diff>
--- a/Arif 0829_8/Arif 0829_8.xlsx
+++ b/Arif 0829_8/Arif 0829_8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Scraping\Don Osterloh\Scraping data\Arif 0829_8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B888422D-044E-454B-AE51-6818BDD2E802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD7A7AE-D6AE-48CC-89C0-CACF5BE43D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="57">
   <si>
     <r>
       <rPr>
@@ -122,16 +122,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Eurostile"/>
-      </rPr>
-      <t>Councillors</t>
-    </r>
-  </si>
-  <si>
     <t>https://alp.org.au/about/organisation</t>
   </si>
   <si>
@@ -268,6 +258,9 @@
   </si>
   <si>
     <t>Mayor</t>
+  </si>
+  <si>
+    <t>Councillors</t>
   </si>
 </sst>
 </file>
@@ -277,12 +270,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000_);[Red]\(0.0000\)"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -455,86 +455,71 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -549,7 +534,25 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -561,25 +564,25 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1077,7 +1080,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1121,19 +1124,19 @@
         <v>20.065000000000001</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" s="19">
         <v>4</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
@@ -1144,19 +1147,19 @@
         <v>20.065100000000001</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="19">
         <v>28</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
@@ -1167,15 +1170,15 @@
         <v>20.065200000000001</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
       <c r="E4" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G4" s="23"/>
       <c r="H4" s="23"/>
@@ -1186,17 +1189,17 @@
         <v>20.065300000000001</v>
       </c>
       <c r="B5" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="29" t="s">
         <v>42</v>
-      </c>
-      <c r="C5" s="29" t="s">
-        <v>43</v>
       </c>
       <c r="D5" s="29"/>
       <c r="E5" s="30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F5" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G5" s="28"/>
       <c r="H5" s="28"/>
@@ -1207,19 +1210,19 @@
         <v>20.0654</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" s="19">
         <v>7</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G6" s="18"/>
       <c r="H6" s="18"/>
@@ -1230,19 +1233,19 @@
         <v>20.0655</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="19">
         <v>6</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G7" s="18"/>
       <c r="H7" s="18"/>
@@ -1253,22 +1256,22 @@
         <v>20.0656</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="19">
         <v>1</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E8" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="18" t="s">
         <v>17</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" s="18" t="s">
-        <v>18</v>
       </c>
       <c r="H8" s="18"/>
       <c r="I8" s="18"/>
@@ -1278,22 +1281,22 @@
         <v>20.0657</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="19">
         <v>2</v>
       </c>
       <c r="D9" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="18" t="s">
         <v>46</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>47</v>
       </c>
       <c r="H9" s="18"/>
       <c r="I9" s="18"/>
@@ -1303,19 +1306,19 @@
         <v>20.065799999999999</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="19">
         <v>119</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G10" s="18"/>
       <c r="H10" s="18"/>
@@ -1326,22 +1329,22 @@
         <v>20.065899999999999</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" s="19">
         <v>22</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="18" t="s">
         <v>23</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="18" t="s">
-        <v>24</v>
       </c>
       <c r="H11" s="18"/>
       <c r="I11" s="18"/>
@@ -1356,11 +1359,11 @@
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="E12" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
@@ -1370,20 +1373,20 @@
         <v>20.066199999999998</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C13" s="19">
         <v>10</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F13" s="18"/>
       <c r="G13" s="36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H13" s="18"/>
       <c r="I13" s="18"/>
@@ -1393,22 +1396,22 @@
         <v>20.0718</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="19">
         <v>13</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H14" s="18"/>
       <c r="I14" s="18"/>
@@ -1418,19 +1421,19 @@
         <v>20.073</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C15" s="19">
         <v>6</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G15" s="18"/>
       <c r="H15" s="18"/>
@@ -1441,12 +1444,12 @@
         <v>20.0731</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
       <c r="E16" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>7</v>
@@ -1460,19 +1463,19 @@
         <v>20.0732</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C17" s="19">
         <v>15</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G17" s="18"/>
       <c r="H17" s="18"/>
@@ -1483,61 +1486,65 @@
         <v>20.0733</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" s="19">
         <v>2</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G18" s="18"/>
       <c r="H18" s="18"/>
       <c r="I18" s="18"/>
     </row>
-    <row r="19" spans="1:9" s="41" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A19" s="37">
+    <row r="19" spans="1:9" s="43" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A19" s="17">
         <v>20.073399999999999</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="19">
+        <v>2</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+    </row>
+    <row r="20" spans="1:9" s="41" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A20" s="37">
+        <v>20.073499999999999</v>
+      </c>
+      <c r="B20" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="40" t="s">
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F19" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
-    </row>
-    <row r="20" spans="1:9" s="9" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A20" s="7">
-        <v>20.073499999999999</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
+      <c r="F20" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
     </row>
     <row r="21" spans="1:9" s="9" customFormat="1" ht="27.75" customHeight="1">
       <c r="A21" s="7">
@@ -1549,7 +1556,7 @@
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
       <c r="E21" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
success task Arif 0829_8 filename 20.0736
</commit_message>
<xml_diff>
--- a/Arif 0829_8/Arif 0829_8.xlsx
+++ b/Arif 0829_8/Arif 0829_8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Scraping\Don Osterloh\Scraping data\Arif 0829_8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD7A7AE-D6AE-48CC-89C0-CACF5BE43D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E754D444-E356-47C2-86B9-8CF19508DFC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="56">
   <si>
     <r>
       <rPr>
@@ -112,16 +112,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Eurostile"/>
-      </rPr>
-      <t>Mayor</t>
-    </r>
-  </si>
-  <si>
     <t>https://alp.org.au/about/organisation</t>
   </si>
   <si>
@@ -270,12 +260,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000_);[Red]\(0.0000\)"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -373,29 +370,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Eurostile"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -455,86 +429,71 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -549,7 +508,25 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -561,25 +538,10 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1080,7 +1042,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1124,19 +1086,19 @@
         <v>20.065000000000001</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="19">
         <v>4</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
@@ -1147,19 +1109,19 @@
         <v>20.065100000000001</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="19">
         <v>28</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
@@ -1170,15 +1132,15 @@
         <v>20.065200000000001</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
       <c r="E4" s="25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G4" s="23"/>
       <c r="H4" s="23"/>
@@ -1189,17 +1151,17 @@
         <v>20.065300000000001</v>
       </c>
       <c r="B5" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="29" t="s">
         <v>41</v>
-      </c>
-      <c r="C5" s="29" t="s">
-        <v>42</v>
       </c>
       <c r="D5" s="29"/>
       <c r="E5" s="30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" s="28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G5" s="28"/>
       <c r="H5" s="28"/>
@@ -1210,19 +1172,19 @@
         <v>20.0654</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="19">
         <v>7</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G6" s="18"/>
       <c r="H6" s="18"/>
@@ -1233,19 +1195,19 @@
         <v>20.0655</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="19">
         <v>6</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G7" s="18"/>
       <c r="H7" s="18"/>
@@ -1256,22 +1218,22 @@
         <v>20.0656</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="19">
         <v>1</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="18" t="s">
         <v>16</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="18" t="s">
-        <v>17</v>
       </c>
       <c r="H8" s="18"/>
       <c r="I8" s="18"/>
@@ -1281,22 +1243,22 @@
         <v>20.0657</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="19">
         <v>2</v>
       </c>
       <c r="D9" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="18" t="s">
         <v>45</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>46</v>
       </c>
       <c r="H9" s="18"/>
       <c r="I9" s="18"/>
@@ -1306,19 +1268,19 @@
         <v>20.065799999999999</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="19">
         <v>119</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G10" s="18"/>
       <c r="H10" s="18"/>
@@ -1329,22 +1291,22 @@
         <v>20.065899999999999</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" s="19">
         <v>22</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E11" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="18" t="s">
         <v>22</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" s="18" t="s">
-        <v>23</v>
       </c>
       <c r="H11" s="18"/>
       <c r="I11" s="18"/>
@@ -1359,11 +1321,11 @@
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="E12" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
@@ -1373,20 +1335,20 @@
         <v>20.066199999999998</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" s="19">
         <v>10</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F13" s="18"/>
       <c r="G13" s="36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H13" s="18"/>
       <c r="I13" s="18"/>
@@ -1396,22 +1358,22 @@
         <v>20.0718</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" s="19">
         <v>13</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H14" s="18"/>
       <c r="I14" s="18"/>
@@ -1421,19 +1383,19 @@
         <v>20.073</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" s="19">
         <v>6</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G15" s="18"/>
       <c r="H15" s="18"/>
@@ -1444,12 +1406,12 @@
         <v>20.0731</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
       <c r="E16" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>7</v>
@@ -1463,107 +1425,115 @@
         <v>20.0732</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C17" s="19">
         <v>15</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G17" s="18"/>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
     </row>
-    <row r="18" spans="1:9" s="42" customFormat="1" ht="27.75" customHeight="1">
+    <row r="18" spans="1:9" s="37" customFormat="1" ht="27.75" customHeight="1">
       <c r="A18" s="17">
         <v>20.0733</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C18" s="19">
         <v>2</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G18" s="18"/>
       <c r="H18" s="18"/>
       <c r="I18" s="18"/>
     </row>
-    <row r="19" spans="1:9" s="43" customFormat="1" ht="27.75" customHeight="1">
+    <row r="19" spans="1:9" s="38" customFormat="1" ht="27.75" customHeight="1">
       <c r="A19" s="17">
         <v>20.073399999999999</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C19" s="19">
         <v>2</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G19" s="18"/>
       <c r="H19" s="18"/>
       <c r="I19" s="18"/>
     </row>
-    <row r="20" spans="1:9" s="41" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A20" s="37">
+    <row r="20" spans="1:9" s="39" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A20" s="17">
         <v>20.073499999999999</v>
       </c>
-      <c r="B20" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="39"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="40" t="s">
+      <c r="B20" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="19">
+        <v>20</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+    </row>
+    <row r="21" spans="1:9" s="39" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A21" s="17">
+        <v>20.073599999999999</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="19">
+        <v>1</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="F20" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-    </row>
-    <row r="21" spans="1:9" s="9" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A21" s="7">
-        <v>20.073599999999999</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
+      <c r="F21" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="11"/>

</xml_diff>

<commit_message>
success task Arif 0829_8 filename 20.0661
</commit_message>
<xml_diff>
--- a/Arif 0829_8/Arif 0829_8.xlsx
+++ b/Arif 0829_8/Arif 0829_8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Scraping\Don Osterloh\Scraping data\Arif 0829_8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E754D444-E356-47C2-86B9-8CF19508DFC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1701D0F8-89FC-45F8-8770-B579DE7F049C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="55">
   <si>
     <r>
       <rPr>
@@ -92,26 +92,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Eurostile"/>
-      </rPr>
-      <t>Names, roles, titles, any PII</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Eurostile"/>
-      </rPr>
-      <t>Our Team</t>
-    </r>
-  </si>
-  <si>
     <t>https://alp.org.au/about/organisation</t>
   </si>
   <si>
@@ -251,6 +231,9 @@
   </si>
   <si>
     <t>Councillors</t>
+  </si>
+  <si>
+    <t>Our Team</t>
   </si>
 </sst>
 </file>
@@ -260,12 +243,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000_);[Red]\(0.0000\)"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -429,86 +419,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -523,7 +480,25 @@
     <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -535,10 +510,10 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1041,16 +1016,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="12" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" style="8" customWidth="1"/>
     <col min="2" max="2" width="40.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="16" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" style="10" customWidth="1"/>
     <col min="5" max="5" width="78.28515625" customWidth="1"/>
     <col min="6" max="6" width="43.42578125" customWidth="1"/>
     <col min="7" max="9" width="16.85546875" customWidth="1"/>
@@ -1081,465 +1056,473 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="21" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A2" s="17">
+    <row r="2" spans="1:9" s="15" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A2" s="11">
         <v>20.065000000000001</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="13">
+        <v>4</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+    </row>
+    <row r="3" spans="1:9" s="15" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A3" s="11">
+        <v>20.065100000000001</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="19">
-        <v>4</v>
-      </c>
-      <c r="D2" s="19" t="s">
+      <c r="C3" s="13">
+        <v>28</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+    </row>
+    <row r="4" spans="1:9" s="20" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A4" s="16">
+        <v>20.065200000000001</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+    </row>
+    <row r="5" spans="1:9" s="25" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A5" s="21">
+        <v>20.065300000000001</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="23"/>
+      <c r="E5" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+    </row>
+    <row r="6" spans="1:9" s="15" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A6" s="11">
+        <v>20.0654</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="13">
+        <v>7</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+    </row>
+    <row r="7" spans="1:9" s="15" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A7" s="11">
+        <v>20.0655</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="13">
+        <v>6</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+    </row>
+    <row r="8" spans="1:9" s="26" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A8" s="11">
+        <v>20.0656</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="13">
+        <v>1</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+    </row>
+    <row r="9" spans="1:9" s="27" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A9" s="11">
+        <v>20.0657</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="13">
+        <v>2</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-    </row>
-    <row r="3" spans="1:9" s="21" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A3" s="17">
-        <v>20.065100000000001</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="19">
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+    </row>
+    <row r="10" spans="1:9" s="28" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A10" s="11">
+        <v>20.065799999999999</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="13">
+        <v>119</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+    </row>
+    <row r="11" spans="1:9" s="29" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A11" s="11">
+        <v>20.065899999999999</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="13">
+        <v>22</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+    </row>
+    <row r="12" spans="1:9" s="34" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A12" s="11">
+        <v>20.066099999999999</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="13">
+        <v>75</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="12"/>
+      <c r="G12" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+    </row>
+    <row r="13" spans="1:9" s="29" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A13" s="11">
+        <v>20.066199999999998</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="13">
+        <v>10</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="12"/>
+      <c r="G13" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+    </row>
+    <row r="14" spans="1:9" s="29" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A14" s="11">
+        <v>20.0718</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="13">
+        <v>13</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+    </row>
+    <row r="15" spans="1:9" s="29" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A15" s="11">
+        <v>20.073</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="13">
+        <v>6</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+    </row>
+    <row r="16" spans="1:9" s="34" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A16" s="11">
+        <v>20.0731</v>
+      </c>
+      <c r="B16" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-    </row>
-    <row r="4" spans="1:9" s="26" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A4" s="22">
-        <v>20.065200000000001</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-    </row>
-    <row r="5" spans="1:9" s="31" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A5" s="27">
-        <v>20.065300000000001</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="29"/>
-      <c r="E5" s="30" t="s">
+      <c r="C16" s="13">
         <v>12</v>
       </c>
-      <c r="F5" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-    </row>
-    <row r="6" spans="1:9" s="21" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A6" s="17">
-        <v>20.0654</v>
-      </c>
-      <c r="B6" s="18" t="s">
+      <c r="D16" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+    </row>
+    <row r="17" spans="1:9" s="29" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A17" s="11">
+        <v>20.0732</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="13">
+        <v>15</v>
+      </c>
+      <c r="D17" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="19">
-        <v>7</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-    </row>
-    <row r="7" spans="1:9" s="21" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A7" s="17">
-        <v>20.0655</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="19">
-        <v>6</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-    </row>
-    <row r="8" spans="1:9" s="32" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A8" s="17">
-        <v>20.0656</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="19">
+      <c r="E17" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+    </row>
+    <row r="18" spans="1:9" s="31" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A18" s="11">
+        <v>20.0733</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="13">
+        <v>2</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+    </row>
+    <row r="19" spans="1:9" s="32" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A19" s="11">
+        <v>20.073399999999999</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="13">
+        <v>2</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+    </row>
+    <row r="20" spans="1:9" s="33" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A20" s="11">
+        <v>20.073499999999999</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="13">
+        <v>20</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+    </row>
+    <row r="21" spans="1:9" s="33" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A21" s="11">
+        <v>20.073599999999999</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="13">
         <v>1</v>
       </c>
-      <c r="D8" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="G8" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-    </row>
-    <row r="9" spans="1:9" s="33" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A9" s="17">
-        <v>20.0657</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="19">
-        <v>2</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-    </row>
-    <row r="10" spans="1:9" s="34" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A10" s="17">
-        <v>20.065799999999999</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="19">
-        <v>119</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-    </row>
-    <row r="11" spans="1:9" s="35" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A11" s="17">
-        <v>20.065899999999999</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="19">
-        <v>22</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-    </row>
-    <row r="12" spans="1:9" s="9" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A12" s="7">
-        <v>20.066099999999999</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-    </row>
-    <row r="13" spans="1:9" s="35" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A13" s="17">
-        <v>20.066199999999998</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="19">
-        <v>10</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="18"/>
-      <c r="G13" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-    </row>
-    <row r="14" spans="1:9" s="35" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A14" s="17">
-        <v>20.0718</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="19">
-        <v>13</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="G14" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-    </row>
-    <row r="15" spans="1:9" s="35" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A15" s="17">
-        <v>20.073</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="19">
-        <v>6</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-    </row>
-    <row r="16" spans="1:9" s="9" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A16" s="7">
-        <v>20.0731</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-    </row>
-    <row r="17" spans="1:9" s="35" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A17" s="17">
-        <v>20.0732</v>
-      </c>
-      <c r="B17" s="18" t="s">
+      <c r="D21" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="19">
-        <v>15</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-    </row>
-    <row r="18" spans="1:9" s="37" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A18" s="17">
-        <v>20.0733</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" s="19">
-        <v>2</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-    </row>
-    <row r="19" spans="1:9" s="38" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A19" s="17">
-        <v>20.073399999999999</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="19">
-        <v>2</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" s="20" t="s">
+      <c r="E21" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-    </row>
-    <row r="20" spans="1:9" s="39" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A20" s="17">
-        <v>20.073499999999999</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="19">
-        <v>20</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-    </row>
-    <row r="21" spans="1:9" s="39" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A21" s="17">
-        <v>20.073599999999999</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" s="19">
-        <v>1</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F21" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
+      <c r="F21" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="11"/>
+      <c r="A22" s="7"/>
       <c r="B22" s="4"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
       <c r="E22" s="5"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>

</xml_diff>

<commit_message>
finisk task Arif 0829_8
</commit_message>
<xml_diff>
--- a/Arif 0829_8/Arif 0829_8.xlsx
+++ b/Arif 0829_8/Arif 0829_8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Scraping\Don Osterloh\Scraping data\Arif 0829_8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1701D0F8-89FC-45F8-8770-B579DE7F049C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06ECA398-22E8-4D76-B82D-38D5C0D706AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -188,9 +188,6 @@
     <t>Federal Management Committee</t>
   </si>
   <si>
-    <t>selenium</t>
-  </si>
-  <si>
     <t>Office Bearers</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>Our Team</t>
+  </si>
+  <si>
+    <t>Sep 03 2023</t>
   </si>
 </sst>
 </file>
@@ -243,7 +243,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000_);[Red]\(0.0000\)"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,6 +315,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Eurostile"/>
@@ -339,13 +346,6 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -357,9 +357,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000716"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Eurostile"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -419,68 +430,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -492,10 +488,13 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -507,12 +506,12 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -520,6 +519,21 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1017,13 +1031,13 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.7109375" style="8" customWidth="1"/>
-    <col min="2" max="2" width="40.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" style="10" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" style="10" customWidth="1"/>
     <col min="5" max="5" width="78.28515625" customWidth="1"/>
@@ -1067,7 +1081,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>7</v>
@@ -1090,7 +1104,7 @@
         <v>28</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>8</v>
@@ -1121,39 +1135,41 @@
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
     </row>
-    <row r="5" spans="1:9" s="25" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A5" s="21">
+    <row r="5" spans="1:9" s="35" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A5" s="31">
         <v>20.065300000000001</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="24" t="s">
+      <c r="C5" s="33">
+        <v>17</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
+      <c r="F5" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
     </row>
     <row r="6" spans="1:9" s="15" customFormat="1" ht="27.75" customHeight="1">
       <c r="A6" s="11">
         <v>20.0654</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="13">
         <v>7</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>11</v>
@@ -1176,7 +1192,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>12</v>
@@ -1188,7 +1204,7 @@
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" s="26" customFormat="1" ht="27.75" customHeight="1">
+    <row r="8" spans="1:9" s="21" customFormat="1" ht="27.75" customHeight="1">
       <c r="A8" s="11">
         <v>20.0656</v>
       </c>
@@ -1199,7 +1215,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E8" s="14" t="s">
         <v>13</v>
@@ -1213,7 +1229,7 @@
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" s="27" customFormat="1" ht="27.75" customHeight="1">
+    <row r="9" spans="1:9" s="22" customFormat="1" ht="27.75" customHeight="1">
       <c r="A9" s="11">
         <v>20.0657</v>
       </c>
@@ -1224,7 +1240,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>17</v>
@@ -1233,23 +1249,23 @@
         <v>35</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:9" s="28" customFormat="1" ht="27.75" customHeight="1">
+    <row r="10" spans="1:9" s="23" customFormat="1" ht="27.75" customHeight="1">
       <c r="A10" s="11">
         <v>20.065799999999999</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="13">
         <v>119</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>18</v>
@@ -1261,18 +1277,18 @@
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
     </row>
-    <row r="11" spans="1:9" s="29" customFormat="1" ht="27.75" customHeight="1">
+    <row r="11" spans="1:9" s="24" customFormat="1" ht="27.75" customHeight="1">
       <c r="A11" s="11">
         <v>20.065899999999999</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="13">
         <v>22</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E11" s="14" t="s">
         <v>19</v>
@@ -1286,53 +1302,53 @@
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
     </row>
-    <row r="12" spans="1:9" s="34" customFormat="1" ht="27.75" customHeight="1">
+    <row r="12" spans="1:9" s="29" customFormat="1" ht="27.75" customHeight="1">
       <c r="A12" s="11">
         <v>20.066099999999999</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" s="13">
         <v>75</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E12" s="14" t="s">
         <v>21</v>
       </c>
       <c r="F12" s="12"/>
-      <c r="G12" s="30" t="s">
+      <c r="G12" s="25" t="s">
         <v>22</v>
       </c>
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
     </row>
-    <row r="13" spans="1:9" s="29" customFormat="1" ht="27.75" customHeight="1">
+    <row r="13" spans="1:9" s="24" customFormat="1" ht="27.75" customHeight="1">
       <c r="A13" s="11">
         <v>20.066199999999998</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" s="13">
         <v>10</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E13" s="14" t="s">
         <v>23</v>
       </c>
       <c r="F13" s="12"/>
-      <c r="G13" s="30" t="s">
+      <c r="G13" s="25" t="s">
         <v>22</v>
       </c>
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
     </row>
-    <row r="14" spans="1:9" s="29" customFormat="1" ht="27.75" customHeight="1">
+    <row r="14" spans="1:9" s="24" customFormat="1" ht="27.75" customHeight="1">
       <c r="A14" s="11">
         <v>20.0718</v>
       </c>
@@ -1343,7 +1359,7 @@
         <v>13</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E14" s="14" t="s">
         <v>24</v>
@@ -1352,23 +1368,23 @@
         <v>35</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:9" s="29" customFormat="1" ht="27.75" customHeight="1">
+    <row r="15" spans="1:9" s="24" customFormat="1" ht="27.75" customHeight="1">
       <c r="A15" s="11">
         <v>20.073</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" s="13">
         <v>6</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E15" s="14" t="s">
         <v>26</v>
@@ -1380,7 +1396,7 @@
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
     </row>
-    <row r="16" spans="1:9" s="34" customFormat="1" ht="27.75" customHeight="1">
+    <row r="16" spans="1:9" s="29" customFormat="1" ht="27.75" customHeight="1">
       <c r="A16" s="11">
         <v>20.0731</v>
       </c>
@@ -1391,7 +1407,7 @@
         <v>12</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E16" s="14" t="s">
         <v>27</v>
@@ -1403,18 +1419,18 @@
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
     </row>
-    <row r="17" spans="1:9" s="29" customFormat="1" ht="27.75" customHeight="1">
+    <row r="17" spans="1:9" s="24" customFormat="1" ht="27.75" customHeight="1">
       <c r="A17" s="11">
         <v>20.0732</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" s="13">
         <v>15</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E17" s="14" t="s">
         <v>29</v>
@@ -1426,18 +1442,18 @@
       <c r="H17" s="12"/>
       <c r="I17" s="12"/>
     </row>
-    <row r="18" spans="1:9" s="31" customFormat="1" ht="27.75" customHeight="1">
+    <row r="18" spans="1:9" s="26" customFormat="1" ht="27.75" customHeight="1">
       <c r="A18" s="11">
         <v>20.0733</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" s="13">
         <v>2</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E18" s="14" t="s">
         <v>30</v>
@@ -1449,18 +1465,18 @@
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
     </row>
-    <row r="19" spans="1:9" s="32" customFormat="1" ht="27.75" customHeight="1">
+    <row r="19" spans="1:9" s="27" customFormat="1" ht="27.75" customHeight="1">
       <c r="A19" s="11">
         <v>20.073399999999999</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C19" s="13">
         <v>2</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E19" s="14" t="s">
         <v>31</v>
@@ -1472,18 +1488,18 @@
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
     </row>
-    <row r="20" spans="1:9" s="33" customFormat="1" ht="27.75" customHeight="1">
+    <row r="20" spans="1:9" s="28" customFormat="1" ht="27.75" customHeight="1">
       <c r="A20" s="11">
         <v>20.073499999999999</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C20" s="13">
         <v>20</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E20" s="14" t="s">
         <v>32</v>
@@ -1495,18 +1511,18 @@
       <c r="H20" s="12"/>
       <c r="I20" s="12"/>
     </row>
-    <row r="21" spans="1:9" s="33" customFormat="1" ht="27.75" customHeight="1">
+    <row r="21" spans="1:9" s="28" customFormat="1" ht="27.75" customHeight="1">
       <c r="A21" s="11">
         <v>20.073599999999999</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C21" s="13">
         <v>1</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E21" s="14" t="s">
         <v>33</v>

</xml_diff>